<commit_message>
adjust scaling of some graphs still need to fix timeline preview
</commit_message>
<xml_diff>
--- a/python_stuff/pneumonia.xlsx
+++ b/python_stuff/pneumonia.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="560" windowWidth="25760" windowHeight="9260" tabRatio="500"/>
+    <workbookView xWindow="2780" yWindow="120" windowWidth="25760" windowHeight="17140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>